<commit_message>
Thu Feb  1 06:50:04 AM CST 2024
</commit_message>
<xml_diff>
--- a/lixiao/summary_2024-1/assess_绩效+软性考核表.xlsx
+++ b/lixiao/summary_2024-1/assess_绩效+软性考核表.xlsx
@@ -2219,10 +2219,8 @@
           <t/>
         </is>
       </c>
-      <c r="K7" s="23" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+      <c r="K7" s="23">
+        <v>0.15</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -2272,10 +2270,8 @@
           <t/>
         </is>
       </c>
-      <c r="K8" s="23" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+      <c r="K8" s="23">
+        <v>0.083</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -2325,10 +2321,8 @@
           <t/>
         </is>
       </c>
-      <c r="K9" s="23" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+      <c r="K9" s="23">
+        <v>0.25</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -2342,7 +2336,7 @@
       </c>
       <c r="C10" s="23" t="inlineStr">
         <is>
-          <t>N2023121805</t>
+          <t>A2023112804</t>
         </is>
       </c>
       <c r="D10" s="23" t="inlineStr">
@@ -2352,7 +2346,7 @@
       </c>
       <c r="E10" s="37" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>sci3-5</t>
         </is>
       </c>
       <c r="F10" s="23">
@@ -2360,7 +2354,7 @@
       </c>
       <c r="G10" s="38" t="inlineStr">
         <is>
-          <t>网络药理学+Mandenol与piezo1分子对接</t>
+          <t>质谱+网络药理学分析</t>
         </is>
       </c>
       <c r="H10" s="39" t="inlineStr">
@@ -2378,10 +2372,8 @@
           <t/>
         </is>
       </c>
-      <c r="K10" s="23" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+      <c r="K10" s="23">
+        <v>0.15</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -2395,7 +2387,7 @@
       </c>
       <c r="C11" s="23" t="inlineStr">
         <is>
-          <t>A2023112804</t>
+          <t>周宇查询学者发文和 H 指数</t>
         </is>
       </c>
       <c r="D11" s="23" t="inlineStr">
@@ -2405,7 +2397,7 @@
       </c>
       <c r="E11" s="37" t="inlineStr">
         <is>
-          <t>sci3-5</t>
+          <t/>
         </is>
       </c>
       <c r="F11" s="23">
@@ -2413,7 +2405,7 @@
       </c>
       <c r="G11" s="38" t="inlineStr">
         <is>
-          <t>质谱+网络药理学分析</t>
+          <t>查询学者发文和 H 指数</t>
         </is>
       </c>
       <c r="H11" s="39" t="inlineStr">
@@ -2431,10 +2423,8 @@
           <t/>
         </is>
       </c>
-      <c r="K11" s="23" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+      <c r="K11" s="23">
+        <v>0.15</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -2448,7 +2438,7 @@
       </c>
       <c r="C12" s="23" t="inlineStr">
         <is>
-          <t>周宇查询学者发文和 H 指数</t>
+          <t>雅威1月业务审核</t>
         </is>
       </c>
       <c r="D12" s="23" t="inlineStr">
@@ -2466,7 +2456,7 @@
       </c>
       <c r="G12" s="38" t="inlineStr">
         <is>
-          <t>查询学者发文和 H 指数</t>
+          <t>雅威1月业务审核</t>
         </is>
       </c>
       <c r="H12" s="39" t="inlineStr">
@@ -2484,10 +2474,8 @@
           <t/>
         </is>
       </c>
-      <c r="K12" s="23" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+      <c r="K12" s="23">
+        <v>0.008</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -2506,7 +2494,7 @@
       </c>
       <c r="D13" s="23" t="inlineStr">
         <is>
-          <t>其他业务</t>
+          <t>固定业务</t>
         </is>
       </c>
       <c r="E13" s="37" t="inlineStr">
@@ -2537,10 +2525,8 @@
           <t/>
         </is>
       </c>
-      <c r="K13" s="23" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+      <c r="K13" s="23">
+        <v>0.25</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -2725,23 +2711,23 @@
         <v>31</v>
       </c>
       <c r="F29" s="43">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G29" s="26" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="H29" s="26" t="e">
-        <v>#N/A</v>
+      <c r="H29" s="26">
+        <v>0.25</v>
       </c>
       <c r="I29" s="51" t="inlineStr">
         <is>
-          <t>NA+NA+NA+NA+NA+NA+NA=NA</t>
-        </is>
-      </c>
-      <c r="J29" s="26" t="e">
-        <v>#N/A</v>
+          <t>0.25=0.25</t>
+        </is>
+      </c>
+      <c r="J29" s="26">
+        <v>1.041</v>
       </c>
       <c r="K29" s="52"/>
     </row>
@@ -2750,11 +2736,21 @@
       <c r="E30" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="43"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="51" t="s">
-        <v>34</v>
+      <c r="F30" s="43">
+        <v>6</v>
+      </c>
+      <c r="G30" s="26" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H30" s="26">
+        <v>0.791</v>
+      </c>
+      <c r="I30" s="51" t="inlineStr">
+        <is>
+          <t>0.15+0.083+0.25+0.15+0.15+0.008=0.791</t>
+        </is>
       </c>
       <c r="J30" s="26"/>
       <c r="K30" s="52"/>

</xml_diff>